<commit_message>
finished code selenium with webdreiver
</commit_message>
<xml_diff>
--- a/seWebDriver.demo/excel/testCaseTienDien.xlsx
+++ b/seWebDriver.demo/excel/testCaseTienDien.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspace\20065161\HK1_23_24\DamBaoChatLuongVaKiemThuPhanMem\seWebDriver.demo\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DDBC88B-0B2D-4F69-9E0B-E5CE8E2FBA91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72756D9D-E432-41D0-B185-15C0AF78E765}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -582,32 +582,32 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1003,8 +1003,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:O39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1021,13 +1021,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="24" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A1" s="42" t="s">
+      <c r="A1" s="38" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="42"/>
-      <c r="C1" s="42"/>
-      <c r="D1" s="42"/>
-      <c r="E1" s="42"/>
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
     </row>
     <row r="2" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="16" t="s">
@@ -1096,7 +1096,7 @@
       <c r="E6" s="21"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" s="38" t="s">
+      <c r="A7" s="40" t="s">
         <v>17</v>
       </c>
       <c r="B7" s="9" t="s">
@@ -1109,7 +1109,7 @@
       <c r="E7" s="12"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8" s="39"/>
+      <c r="A8" s="41"/>
       <c r="B8" s="5" t="s">
         <v>19</v>
       </c>
@@ -1120,7 +1120,7 @@
       <c r="E8" s="13"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" s="39"/>
+      <c r="A9" s="41"/>
       <c r="B9" s="5" t="s">
         <v>20</v>
       </c>
@@ -1131,7 +1131,7 @@
       <c r="E9" s="13"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" s="39"/>
+      <c r="A10" s="41"/>
       <c r="B10" s="5" t="s">
         <v>21</v>
       </c>
@@ -1142,7 +1142,7 @@
       <c r="E10" s="13"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11" s="39"/>
+      <c r="A11" s="41"/>
       <c r="B11" s="5" t="s">
         <v>22</v>
       </c>
@@ -1153,7 +1153,7 @@
       <c r="E11" s="13"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12" s="39"/>
+      <c r="A12" s="41"/>
       <c r="B12" s="5" t="s">
         <v>26</v>
       </c>
@@ -1164,7 +1164,7 @@
       <c r="E12" s="13"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A13" s="39"/>
+      <c r="A13" s="41"/>
       <c r="B13" s="5"/>
       <c r="C13" s="3"/>
       <c r="D13" s="3">
@@ -1173,7 +1173,7 @@
       <c r="E13" s="13"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A14" s="39"/>
+      <c r="A14" s="41"/>
       <c r="B14" s="5"/>
       <c r="C14" s="3"/>
       <c r="D14" s="3">
@@ -1182,7 +1182,7 @@
       <c r="E14" s="13"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A15" s="39"/>
+      <c r="A15" s="41"/>
       <c r="B15" s="5"/>
       <c r="C15" s="3"/>
       <c r="D15" s="3">
@@ -1191,7 +1191,7 @@
       <c r="E15" s="13"/>
     </row>
     <row r="16" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="44"/>
+      <c r="A16" s="42"/>
       <c r="B16" s="10"/>
       <c r="C16" s="11"/>
       <c r="D16" s="11">
@@ -1200,13 +1200,13 @@
       <c r="E16" s="14"/>
     </row>
     <row r="17" spans="1:15" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="A17" s="43" t="s">
+      <c r="A17" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="B17" s="43"/>
-      <c r="C17" s="43"/>
-      <c r="D17" s="43"/>
-      <c r="E17" s="43"/>
+      <c r="B17" s="39"/>
+      <c r="C17" s="39"/>
+      <c r="D17" s="39"/>
+      <c r="E17" s="39"/>
       <c r="F17" s="26"/>
       <c r="G17" s="26"/>
       <c r="H17" s="26"/>
@@ -1238,13 +1238,13 @@
       <c r="I18" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="J18" s="45" t="s">
+      <c r="J18" s="43" t="s">
         <v>28</v>
       </c>
-      <c r="K18" s="46"/>
+      <c r="K18" s="44"/>
     </row>
     <row r="19" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="38" t="s">
+      <c r="A19" s="40" t="s">
         <v>11</v>
       </c>
       <c r="B19" s="33">
@@ -1284,7 +1284,7 @@
       <c r="O19" s="7"/>
     </row>
     <row r="20" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="39"/>
+      <c r="A20" s="41"/>
       <c r="B20" s="3">
         <v>2</v>
       </c>
@@ -1321,7 +1321,7 @@
       <c r="N20" s="7"/>
     </row>
     <row r="21" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="39"/>
+      <c r="A21" s="41"/>
       <c r="B21" s="3">
         <v>3</v>
       </c>
@@ -1358,7 +1358,7 @@
       <c r="N21" s="7"/>
     </row>
     <row r="22" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="39"/>
+      <c r="A22" s="41"/>
       <c r="B22" s="3">
         <v>4</v>
       </c>
@@ -1395,7 +1395,7 @@
       <c r="N22" s="4"/>
     </row>
     <row r="23" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="39"/>
+      <c r="A23" s="41"/>
       <c r="B23" s="3">
         <v>5</v>
       </c>
@@ -1432,7 +1432,7 @@
       <c r="N23" s="4"/>
     </row>
     <row r="24" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="39"/>
+      <c r="A24" s="41"/>
       <c r="B24" s="20">
         <v>6</v>
       </c>
@@ -1469,7 +1469,7 @@
       <c r="N24" s="4"/>
     </row>
     <row r="25" spans="1:15" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="38" t="s">
+      <c r="A25" s="40" t="s">
         <v>16</v>
       </c>
       <c r="B25" s="15">
@@ -1498,7 +1498,7 @@
       <c r="J25" s="36"/>
     </row>
     <row r="26" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="39"/>
+      <c r="A26" s="41"/>
       <c r="B26" s="3">
         <v>8</v>
       </c>
@@ -1524,7 +1524,7 @@
       </c>
     </row>
     <row r="27" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="39"/>
+      <c r="A27" s="41"/>
       <c r="B27" s="20">
         <v>9</v>
       </c>
@@ -1550,7 +1550,7 @@
       </c>
     </row>
     <row r="28" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="38" t="s">
+      <c r="A28" s="40" t="s">
         <v>12</v>
       </c>
       <c r="B28" s="15">
@@ -1582,7 +1582,7 @@
       </c>
     </row>
     <row r="29" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="39"/>
+      <c r="A29" s="41"/>
       <c r="B29" s="3">
         <v>11</v>
       </c>
@@ -1612,7 +1612,7 @@
       </c>
     </row>
     <row r="30" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="39"/>
+      <c r="A30" s="41"/>
       <c r="B30" s="3">
         <v>12</v>
       </c>
@@ -1642,7 +1642,7 @@
       </c>
     </row>
     <row r="31" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="39"/>
+      <c r="A31" s="41"/>
       <c r="B31" s="3">
         <v>13</v>
       </c>
@@ -1672,7 +1672,7 @@
       </c>
     </row>
     <row r="32" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="39"/>
+      <c r="A32" s="41"/>
       <c r="B32" s="3">
         <v>14</v>
       </c>
@@ -1702,7 +1702,7 @@
       </c>
     </row>
     <row r="33" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="39"/>
+      <c r="A33" s="41"/>
       <c r="B33" s="3">
         <v>15</v>
       </c>
@@ -1732,7 +1732,7 @@
       </c>
     </row>
     <row r="34" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="39"/>
+      <c r="A34" s="41"/>
       <c r="B34" s="3">
         <v>16</v>
       </c>
@@ -1762,7 +1762,7 @@
       </c>
     </row>
     <row r="35" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="39"/>
+      <c r="A35" s="41"/>
       <c r="B35" s="3">
         <v>17</v>
       </c>
@@ -1792,7 +1792,7 @@
       </c>
     </row>
     <row r="36" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="39"/>
+      <c r="A36" s="41"/>
       <c r="B36" s="3">
         <v>18</v>
       </c>
@@ -1822,7 +1822,7 @@
       </c>
     </row>
     <row r="37" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="39"/>
+      <c r="A37" s="41"/>
       <c r="B37" s="20">
         <v>19</v>
       </c>
@@ -1852,7 +1852,7 @@
       </c>
     </row>
     <row r="38" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A38" s="40" t="s">
+      <c r="A38" s="45" t="s">
         <v>13</v>
       </c>
       <c r="B38" s="15">
@@ -1880,7 +1880,7 @@
       </c>
     </row>
     <row r="39" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A39" s="41"/>
+      <c r="A39" s="46"/>
       <c r="B39" s="11">
         <v>21</v>
       </c>
@@ -1907,14 +1907,14 @@
     </row>
   </sheetData>
   <mergeCells count="8">
-    <mergeCell ref="J18:K18"/>
-    <mergeCell ref="A19:A24"/>
     <mergeCell ref="A25:A27"/>
     <mergeCell ref="A28:A37"/>
     <mergeCell ref="A38:A39"/>
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="A17:E17"/>
     <mergeCell ref="A7:A16"/>
+    <mergeCell ref="J18:K18"/>
+    <mergeCell ref="A19:A24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>